<commit_message>
Added support for excel config files as well
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -1,13 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eyash\Documents\UiPath\GLamework\Config\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F86C63C-CD97-4AC5-97C4-8F90E6733AC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="36890" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="assets" sheetId="2" r:id="rId1"/>
+    <sheet name="credentials" sheetId="3" r:id="rId2"/>
+    <sheet name="settings" sheetId="4" r:id="rId3"/>
+    <sheet name="systemExceptions" sheetId="5" r:id="rId4"/>
+    <sheet name="businessExceptions" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,8 +28,214 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="67">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>_useLocalValues</t>
+  </si>
+  <si>
+    <t>mailServer</t>
+  </si>
+  <si>
+    <t>ITEmail</t>
+  </si>
+  <si>
+    <t>BusinessEmail</t>
+  </si>
+  <si>
+    <t>ScreenshotPath</t>
+  </si>
+  <si>
+    <t>outlook365.office.com</t>
+  </si>
+  <si>
+    <t>it@domain.com</t>
+  </si>
+  <si>
+    <t>business@domain.com</t>
+  </si>
+  <si>
+    <t>webapp1</t>
+  </si>
+  <si>
+    <t>process.queue</t>
+  </si>
+  <si>
+    <t>process.name</t>
+  </si>
+  <si>
+    <t>process.readOnlyMode</t>
+  </si>
+  <si>
+    <t>process.howToAddStringsInConfig</t>
+  </si>
+  <si>
+    <t>network.retryCount.med</t>
+  </si>
+  <si>
+    <t>network.retryCount.low</t>
+  </si>
+  <si>
+    <t>network.retryCount.high</t>
+  </si>
+  <si>
+    <t>network.retryTimeout.low</t>
+  </si>
+  <si>
+    <t>network.retryTimeout.med</t>
+  </si>
+  <si>
+    <t>network.retryTimeout.high</t>
+  </si>
+  <si>
+    <t>framework.enableDispatcherLoop</t>
+  </si>
+  <si>
+    <t>framework.dispatchMode</t>
+  </si>
+  <si>
+    <t>framework.testDataPath</t>
+  </si>
+  <si>
+    <t>framework.maintenanceStart</t>
+  </si>
+  <si>
+    <t>framework.maintenanceEnd</t>
+  </si>
+  <si>
+    <t>framework.failJobOnScreenshot</t>
+  </si>
+  <si>
+    <t>initialize.id</t>
+  </si>
+  <si>
+    <t>initialize.delay</t>
+  </si>
+  <si>
+    <t>initialize.max</t>
+  </si>
+  <si>
+    <t>initialize.email.to</t>
+  </si>
+  <si>
+    <t>initialize.email.subject</t>
+  </si>
+  <si>
+    <t>initialize.email.body</t>
+  </si>
+  <si>
+    <t>performer.id</t>
+  </si>
+  <si>
+    <t>dispatcher.id</t>
+  </si>
+  <si>
+    <t>dispatcher.delay</t>
+  </si>
+  <si>
+    <t>dispatcher.max</t>
+  </si>
+  <si>
+    <t>dispatcher.email.to</t>
+  </si>
+  <si>
+    <t>dispatcher.email.subject</t>
+  </si>
+  <si>
+    <t>dispatcher.email.body</t>
+  </si>
+  <si>
+    <t>performer.max</t>
+  </si>
+  <si>
+    <t>FrameworkQueue</t>
+  </si>
+  <si>
+    <t>GLamework</t>
+  </si>
+  <si>
+    <t>${settings.process.queue + `: ` + settings.process.name}</t>
+  </si>
+  <si>
+    <t>00:00:05</t>
+  </si>
+  <si>
+    <t>00:00:02</t>
+  </si>
+  <si>
+    <t>00:00:10</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>2:00:00</t>
+  </si>
+  <si>
+    <t>4:00:00</t>
+  </si>
+  <si>
+    <t>initialize</t>
+  </si>
+  <si>
+    <t>00:15:00</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>${assets.ITEmail}</t>
+  </si>
+  <si>
+    <t>perform</t>
+  </si>
+  <si>
+    <t>dispatch</t>
+  </si>
+  <si>
+    <t>dispatcher.invalidMode</t>
+  </si>
+  <si>
+    <t>handleStateExceptions.invalidRoute</t>
+  </si>
+  <si>
+    <t>Invalid framework.dispatchMode: QA, PROD</t>
+  </si>
+  <si>
+    <t>HandleStateExceptions encountered an unexpected state.</t>
+  </si>
+  <si>
+    <t>step2.exception2</t>
+  </si>
+  <si>
+    <t>step1.exception1</t>
+  </si>
+  <si>
+    <t>Message for exception 1</t>
+  </si>
+  <si>
+    <t>Message for exception 2</t>
+  </si>
+  <si>
+    <t>Data\\test.xlsx</t>
+  </si>
+  <si>
+    <t>Screenshots\\</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +546,459 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C3098F-1EC8-47AF-8306-9CE11C4F33CD}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{6DDD4438-5898-4776-93B9-F27C6ADD4588}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{E89CC42A-EB05-4BD6-80EF-B7369D03DCD0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455FEF03-7BAD-4345-8BE9-0D03106E5486}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BA5D446-B129-4963-8F78-4F3027E12AC8}">
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C7B85E4-FA3A-40FB-9DBB-E3B0609E55E3}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{907222D4-71D4-475E-82C3-AE2C1755E13C}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>